<commit_message>
added .gitignore, deleted unnecessary files, added environment file, add RunSingleCase notebook
</commit_message>
<xml_diff>
--- a/watertap3/watertap3/data/treatment_train_setup.xlsx
+++ b/watertap3/watertap3/data/treatment_train_setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ksitterl/Documents/Python/watertap3/NAWI-WaterTAP3/watertap3/watertap3/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4759C2B2-C9C9-2C4B-8BDD-AB5538A05FD7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577954AB-9C22-0B4B-8C08-797C27B2BD14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19940" windowHeight="21600" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
+    <workbookView xWindow="5940" yWindow="460" windowWidth="25940" windowHeight="21140" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="2" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7738" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7738" uniqueCount="652">
   <si>
     <t>outlet</t>
   </si>
@@ -1981,9 +1981,6 @@
   </si>
   <si>
     <t>solaire_s</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>include electricity cost for pump (pumping_station if no cost for pump_active and pump_restore)</t>
@@ -2565,8 +2562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A817730-1204-A546-BE57-7C8F485A64DC}">
   <dimension ref="A1:Z1466"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I962" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I980" sqref="I980"/>
+    <sheetView tabSelected="1" topLeftCell="E405" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G421" sqref="G421"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16389,7 +16386,7 @@
         <v>71</v>
       </c>
       <c r="G417" s="7" t="s">
-        <v>475</v>
+        <v>52</v>
       </c>
       <c r="H417" s="7" t="s">
         <v>0</v>
@@ -16400,7 +16397,7 @@
     </row>
     <row r="418" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A418" s="7" t="s">
-        <v>628</v>
+        <v>400</v>
       </c>
       <c r="B418" s="7" t="s">
         <v>111</v>
@@ -16430,7 +16427,7 @@
     </row>
     <row r="419" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A419" s="7" t="s">
-        <v>628</v>
+        <v>400</v>
       </c>
       <c r="B419" s="7" t="s">
         <v>111</v>
@@ -16459,7 +16456,7 @@
     </row>
     <row r="420" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A420" s="7" t="s">
-        <v>628</v>
+        <v>400</v>
       </c>
       <c r="B420" s="7" t="s">
         <v>111</v>
@@ -17612,7 +17609,7 @@
     </row>
     <row r="469" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C469" s="13" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="470" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -17635,7 +17632,7 @@
         <v>177</v>
       </c>
       <c r="G470" s="7" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="H470" s="7" t="s">
         <v>0</v>
@@ -17661,12 +17658,12 @@
         <v>23</v>
       </c>
       <c r="F471" s="7" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G471" s="7"/>
       <c r="H471" s="7"/>
       <c r="I471" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="472" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -17686,7 +17683,7 @@
         <v>22</v>
       </c>
       <c r="F472" s="7" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G472" s="2" t="s">
         <v>413</v>
@@ -17718,7 +17715,7 @@
         <v>413</v>
       </c>
       <c r="G473" s="7" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="H473" s="7" t="s">
         <v>28</v>
@@ -17744,7 +17741,7 @@
         <v>575</v>
       </c>
       <c r="G474" s="7" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="H474" s="7" t="s">
         <v>28</v>
@@ -17770,16 +17767,16 @@
         <v>22</v>
       </c>
       <c r="F475" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="G475" s="7" t="s">
         <v>635</v>
-      </c>
-      <c r="G475" s="7" t="s">
-        <v>636</v>
       </c>
       <c r="H475" s="7" t="s">
         <v>383</v>
       </c>
       <c r="I475" s="7" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="476" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -17799,7 +17796,7 @@
         <v>22</v>
       </c>
       <c r="F476" s="7" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G476" s="7" t="s">
         <v>43</v>
@@ -17831,7 +17828,7 @@
         <v>178</v>
       </c>
       <c r="G477" s="7" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="H477" s="7" t="s">
         <v>0</v>
@@ -17857,7 +17854,7 @@
         <v>22</v>
       </c>
       <c r="F478" s="7" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="G478" s="7" t="s">
         <v>179</v>
@@ -17889,7 +17886,7 @@
         <v>179</v>
       </c>
       <c r="G479" s="7" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="H479" s="7" t="s">
         <v>28</v>
@@ -17940,7 +17937,7 @@
         <v>23</v>
       </c>
       <c r="F481" s="7" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="G481" s="19"/>
       <c r="H481" s="19"/>
@@ -17960,7 +17957,7 @@
     </row>
     <row r="483" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A483" s="7" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B483" s="7" t="s">
         <v>111</v>
@@ -17978,7 +17975,7 @@
         <v>177</v>
       </c>
       <c r="G483" s="7" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="H483" s="7" t="s">
         <v>0</v>
@@ -17989,7 +17986,7 @@
     </row>
     <row r="484" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A484" s="7" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B484" s="7" t="s">
         <v>111</v>
@@ -18004,21 +18001,21 @@
         <v>22</v>
       </c>
       <c r="F484" s="7" t="s">
+        <v>630</v>
+      </c>
+      <c r="G484" s="7" t="s">
+        <v>629</v>
+      </c>
+      <c r="H484" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I484" s="2" t="s">
         <v>631</v>
-      </c>
-      <c r="G484" s="7" t="s">
-        <v>630</v>
-      </c>
-      <c r="H484" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I484" s="2" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="485" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A485" s="7" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B485" s="7" t="s">
         <v>111</v>
@@ -18033,7 +18030,7 @@
         <v>22</v>
       </c>
       <c r="F485" s="7" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G485" s="2" t="s">
         <v>413</v>
@@ -18047,7 +18044,7 @@
     </row>
     <row r="486" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A486" s="7" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B486" s="7" t="s">
         <v>111</v>
@@ -18065,7 +18062,7 @@
         <v>413</v>
       </c>
       <c r="G486" s="7" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="H486" s="7" t="s">
         <v>28</v>
@@ -18073,7 +18070,7 @@
     </row>
     <row r="487" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A487" s="7" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B487" s="7" t="s">
         <v>111</v>
@@ -18091,7 +18088,7 @@
         <v>575</v>
       </c>
       <c r="G487" s="7" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="H487" s="7" t="s">
         <v>28</v>
@@ -18102,7 +18099,7 @@
     </row>
     <row r="488" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A488" s="7" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B488" s="7" t="s">
         <v>111</v>
@@ -18117,21 +18114,21 @@
         <v>22</v>
       </c>
       <c r="F488" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="G488" s="7" t="s">
         <v>635</v>
-      </c>
-      <c r="G488" s="7" t="s">
-        <v>636</v>
       </c>
       <c r="H488" s="7" t="s">
         <v>383</v>
       </c>
       <c r="I488" s="7" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="489" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A489" s="7" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B489" s="7" t="s">
         <v>111</v>
@@ -18146,7 +18143,7 @@
         <v>22</v>
       </c>
       <c r="F489" s="7" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G489" s="7" t="s">
         <v>43</v>
@@ -18160,7 +18157,7 @@
     </row>
     <row r="490" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A490" s="7" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B490" s="7" t="s">
         <v>111</v>
@@ -18178,7 +18175,7 @@
         <v>178</v>
       </c>
       <c r="G490" s="7" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="H490" s="7" t="s">
         <v>0</v>
@@ -18189,7 +18186,7 @@
     </row>
     <row r="491" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A491" s="7" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B491" s="7" t="s">
         <v>111</v>
@@ -18204,7 +18201,7 @@
         <v>22</v>
       </c>
       <c r="F491" s="7" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="G491" s="7" t="s">
         <v>179</v>
@@ -18218,7 +18215,7 @@
     </row>
     <row r="492" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A492" s="7" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B492" s="7" t="s">
         <v>111</v>
@@ -18236,7 +18233,7 @@
         <v>179</v>
       </c>
       <c r="G492" s="7" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="H492" s="7" t="s">
         <v>28</v>
@@ -18247,7 +18244,7 @@
     </row>
     <row r="493" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A493" s="7" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B493" s="7" t="s">
         <v>111</v>
@@ -18272,7 +18269,7 @@
     </row>
     <row r="494" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A494" s="7" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B494" s="7" t="s">
         <v>111</v>
@@ -18287,7 +18284,7 @@
         <v>23</v>
       </c>
       <c r="F494" s="7" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="G494" s="19"/>
       <c r="H494" s="19"/>
@@ -26646,7 +26643,7 @@
     </row>
     <row r="821" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A821" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B821" s="2" t="s">
         <v>111</v>
@@ -26692,7 +26689,7 @@
     </row>
     <row r="822" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A822" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B822" s="2" t="s">
         <v>111</v>
@@ -26738,7 +26735,7 @@
     </row>
     <row r="823" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A823" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B823" s="2" t="s">
         <v>111</v>
@@ -26784,7 +26781,7 @@
     </row>
     <row r="824" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A824" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B824" s="2" t="s">
         <v>111</v>
@@ -26830,7 +26827,7 @@
     </row>
     <row r="825" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A825" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B825" s="2" t="s">
         <v>111</v>
@@ -26876,7 +26873,7 @@
     </row>
     <row r="826" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A826" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B826" s="2" t="s">
         <v>111</v>
@@ -26922,7 +26919,7 @@
     </row>
     <row r="827" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A827" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B827" s="2" t="s">
         <v>111</v>
@@ -26968,7 +26965,7 @@
     </row>
     <row r="828" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A828" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B828" s="2" t="s">
         <v>111</v>
@@ -27014,7 +27011,7 @@
     </row>
     <row r="829" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A829" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B829" s="2" t="s">
         <v>111</v>
@@ -27060,7 +27057,7 @@
     </row>
     <row r="830" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A830" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B830" s="2" t="s">
         <v>111</v>
@@ -27106,7 +27103,7 @@
     </row>
     <row r="831" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A831" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B831" s="2" t="s">
         <v>111</v>
@@ -27152,7 +27149,7 @@
     </row>
     <row r="832" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A832" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B832" s="2" t="s">
         <v>111</v>
@@ -27198,7 +27195,7 @@
     </row>
     <row r="833" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A833" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B833" s="2" t="s">
         <v>111</v>
@@ -27244,7 +27241,7 @@
     </row>
     <row r="834" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A834" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B834" s="2" t="s">
         <v>111</v>
@@ -27284,7 +27281,7 @@
     </row>
     <row r="835" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A835" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B835" s="2" t="s">
         <v>111</v>
@@ -27324,7 +27321,7 @@
     </row>
     <row r="836" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A836" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B836" s="2" t="s">
         <v>111</v>
@@ -27364,7 +27361,7 @@
     </row>
     <row r="837" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A837" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B837" s="2" t="s">
         <v>111</v>
@@ -27536,7 +27533,7 @@
         <v>383</v>
       </c>
       <c r="I841" s="7" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J841"/>
       <c r="K841"/>
@@ -27717,7 +27714,7 @@
         <v>0</v>
       </c>
       <c r="I845" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J845"/>
       <c r="K845"/>
@@ -27803,13 +27800,13 @@
         <v>75</v>
       </c>
       <c r="G847" s="25" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="H847" s="25" t="s">
         <v>94</v>
       </c>
       <c r="I847" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J847"/>
       <c r="K847"/>
@@ -27855,7 +27852,7 @@
         <v>94</v>
       </c>
       <c r="I848" s="7" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J848"/>
       <c r="K848"/>
@@ -28537,7 +28534,7 @@
         <v>75</v>
       </c>
       <c r="G864" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="H864" s="2" t="s">
         <v>383</v>
@@ -28583,13 +28580,13 @@
         <v>579</v>
       </c>
       <c r="G865" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="H865" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I865" s="7" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J865"/>
       <c r="K865"/>
@@ -29121,7 +29118,7 @@
         <v>0</v>
       </c>
       <c r="I878" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J878"/>
       <c r="K878"/>
@@ -30144,7 +30141,7 @@
         <v>0</v>
       </c>
       <c r="I902" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J902"/>
       <c r="K902"/>
@@ -31023,7 +31020,7 @@
         <v>0</v>
       </c>
       <c r="I928" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="929" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -32517,7 +32514,7 @@
         <v>0</v>
       </c>
       <c r="I983" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="984" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -32788,7 +32785,7 @@
         <v>392</v>
       </c>
       <c r="G996" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H996" s="8" t="s">
         <v>0</v>
@@ -32811,7 +32808,7 @@
         <v>22</v>
       </c>
       <c r="F997" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G997" s="2" t="s">
         <v>314</v>
@@ -32820,7 +32817,7 @@
         <v>0</v>
       </c>
       <c r="I997" s="2" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="998" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>